<commit_message>
summary of the video feature added
</commit_message>
<xml_diff>
--- a/backend/extracted_names.xlsx
+++ b/backend/extracted_names.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,36 +448,396 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>John</t>
+          <t>First1</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Doe</t>
+          <t>Last1</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Jane</t>
+          <t>First2</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Smith</t>
+          <t>Last2</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Bob</t>
+          <t>First3</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Johnson</t>
+          <t>Last3</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>First4</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Last4</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>First5</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Last5</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>First6</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Last6</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>First7</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Last7</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>First8</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Last8</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>First9</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Last9</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>First10</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Last10</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>First11</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Last11</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>First12</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Last12</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>First13</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Last13</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>First14</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Last14</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>First15</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Last15</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>First16</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Last16</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>First17</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Last17</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>First18</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Last18</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>First19</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Last19</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>First20</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Last20</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>First21</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Last21</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>First22</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Last22</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>First23</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Last23</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>First24</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Last24</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>First25</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Last25</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>First26</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Last26</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>First27</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Last27</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>First28</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Last28</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>First29</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Last29</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>First30</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Last30</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>First31</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Last31</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>First32</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Last32</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>First33</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Last33</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
added comments for better readability
</commit_message>
<xml_diff>
--- a/backend/extracted_names.xlsx
+++ b/backend/extracted_names.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,396 +448,36 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>First1</t>
+          <t>John</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Last1</t>
+          <t>Doe</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>First2</t>
+          <t>Jane</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Last2</t>
+          <t>Smith</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>First3</t>
+          <t>Bob</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Last3</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>First4</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Last4</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>First5</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Last5</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>First6</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Last6</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>First7</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Last7</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>First8</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Last8</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>First9</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Last9</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>First10</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Last10</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>First11</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Last11</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>First12</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Last12</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>First13</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Last13</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>First14</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Last14</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>First15</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Last15</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>First16</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Last16</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>First17</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Last17</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>First18</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Last18</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>First19</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>Last19</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>First20</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>Last20</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>First21</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>Last21</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>First22</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>Last22</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>First23</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>Last23</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>First24</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>Last24</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>First25</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>Last25</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>First26</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>Last26</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>First27</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>Last27</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>First28</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>Last28</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>First29</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>Last29</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>First30</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>Last30</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>First31</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>Last31</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>First32</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>Last32</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>First33</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>Last33</t>
+          <t>Johnson</t>
         </is>
       </c>
     </row>

</xml_diff>